<commit_message>
Updated team report to project status as of 2.09.18
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28b3348db4141b85/Documents/Stevens Institue of Technology/Classes/Semester 2/SSW 555 - Agile Methods for Software Development/Assignments/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{D77EC34B-36A3-48B9-998B-7DD4AD767985}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{37CD40BC-DBA3-433E-8FD9-F8F7EAC2C534}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="8963" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,6 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sprint1!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Stories!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
@@ -40,19 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="214">
-  <si>
-    <t>Find marriage date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compare marriage date to birth date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="204">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -158,22 +146,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>gh(at)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh(hm)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Story ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -186,34 +158,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Sprint</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Store birth date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Store death date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compare birth and death dates</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Find marriage record for individual</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Review Results</t>
   </si>
   <si>
@@ -229,15 +177,6 @@
     <t>GitHub Repository:</t>
   </si>
   <si>
-    <t>Bring pizza to our meetings</t>
-  </si>
-  <si>
-    <t>Leaving leftover pizza on the counter</t>
-  </si>
-  <si>
-    <t>Bring silverware for everyone</t>
-  </si>
-  <si>
     <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
   </si>
   <si>
@@ -601,24 +540,6 @@
     <t>US42</t>
   </si>
   <si>
-    <t>T03.01</t>
-  </si>
-  <si>
-    <t>T03.02</t>
-  </si>
-  <si>
-    <t>T03.03</t>
-  </si>
-  <si>
-    <t>T05.01</t>
-  </si>
-  <si>
-    <t>T05.02</t>
-  </si>
-  <si>
-    <t>T05.03</t>
-  </si>
-  <si>
     <t>Dates before current date</t>
   </si>
   <si>
@@ -725,6 +646,42 @@
   </si>
   <si>
     <t>Google hangouts/phone</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>T0.0</t>
+  </si>
+  <si>
+    <t>DC/NO</t>
+  </si>
+  <si>
+    <t>develop date conversion method to be used in stories for this sprint</t>
+  </si>
+  <si>
+    <t>Est Size (LOC)</t>
+  </si>
+  <si>
+    <t>Est Time (mins)</t>
+  </si>
+  <si>
+    <t>Act Size (LOC)</t>
+  </si>
+  <si>
+    <t>Act Time (mins)</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Database:</t>
+  </si>
+  <si>
+    <t>sqLite3</t>
   </si>
 </sst>
 </file>
@@ -987,8 +944,70 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2067,94 +2086,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.46875" customWidth="1"/>
-    <col min="3" max="3" width="9.64453125" customWidth="1"/>
-    <col min="4" max="4" width="20.46875" customWidth="1"/>
-    <col min="5" max="5" width="47.41015625" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.4609375" customWidth="1"/>
+    <col min="3" max="3" width="9.61328125" customWidth="1"/>
+    <col min="4" max="4" width="20.4609375" customWidth="1"/>
+    <col min="5" max="5" width="47.3828125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D11" s="18" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D12" s="18" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>212</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2175,199 +2202,199 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.87890625" customWidth="1"/>
-    <col min="2" max="2" width="22.5859375" customWidth="1"/>
-    <col min="3" max="3" width="38.17578125" customWidth="1"/>
-    <col min="4" max="4" width="8.05859375" customWidth="1"/>
-    <col min="5" max="5" width="7.64453125" customWidth="1"/>
+    <col min="1" max="1" width="8.84375" customWidth="1"/>
+    <col min="2" max="2" width="22.61328125" customWidth="1"/>
+    <col min="3" max="3" width="38.15234375" customWidth="1"/>
+    <col min="4" max="4" width="8.07421875" customWidth="1"/>
+    <col min="5" max="5" width="7.61328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2390,72 +2417,72 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="7"/>
-    <col min="2" max="2" width="9.46875" customWidth="1"/>
-    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3515625" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="7"/>
+    <col min="2" max="2" width="9.4609375" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3828125" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2471,7 +2498,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -2496,7 +2523,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -2521,7 +2548,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -2546,7 +2573,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -2580,38 +2607,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="2"/>
-    <col min="2" max="2" width="16.64453125" customWidth="1"/>
-    <col min="3" max="3" width="12.46875" customWidth="1"/>
-    <col min="4" max="4" width="7.17578125" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="2"/>
+    <col min="2" max="2" width="16.61328125" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2652,174 +2679,159 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.64453125" customWidth="1"/>
-    <col min="2" max="2" width="24.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.64453125" customWidth="1"/>
-    <col min="5" max="5" width="9.29296875" customWidth="1"/>
-    <col min="6" max="6" width="9.52734375" customWidth="1"/>
-    <col min="7" max="7" width="9.87890625" customWidth="1"/>
-    <col min="8" max="8" width="11.05859375" customWidth="1"/>
-    <col min="9" max="9" width="10.8203125" style="6"/>
+    <col min="1" max="1" width="7.61328125" customWidth="1"/>
+    <col min="2" max="2" width="29.23046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.61328125" customWidth="1"/>
+    <col min="5" max="5" width="13.3828125" customWidth="1"/>
+    <col min="6" max="6" width="15.84375" customWidth="1"/>
+    <col min="7" max="7" width="20.23046875" customWidth="1"/>
+    <col min="8" max="8" width="21.53515625" customWidth="1"/>
+    <col min="9" max="9" width="14.69140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>16</v>
+        <v>197</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
+        <v>195</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>201</v>
       </c>
       <c r="E2">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="F2">
-        <v>60</v>
-      </c>
-      <c r="G2">
-        <v>120</v>
-      </c>
-      <c r="H2">
-        <v>90</v>
-      </c>
-      <c r="I2" s="6">
-        <v>40444</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>192</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8">
-        <v>200</v>
-      </c>
-      <c r="F8">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>177</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
+        <v>193</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7">
+        <v>65</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2828,33 +2840,47 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{2DCD5CA0-4A5A-4BD1-984B-70D227AFE942}"/>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Incomplete">
+      <formula>NOT(ISERROR(SEARCH("Incomplete",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{06A7FB0F-FD25-4481-873C-BCA5B754C452}">
+            <xm:f>NOT(ISERROR(SEARCH("Complete",D1)))</xm:f>
+            <xm:f>"Complete"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2866,35 +2892,35 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2912,35 +2938,35 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2957,35 +2983,35 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3003,37 +3029,37 @@
       <selection pane="bottomLeft" activeCell="A19" sqref="A19:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.234375" customWidth="1"/>
-    <col min="2" max="2" width="30.76171875" customWidth="1"/>
-    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.23046875" customWidth="1"/>
+    <col min="2" max="2" width="30.765625" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3041,13 +3067,13 @@
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3055,13 +3081,13 @@
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3069,13 +3095,13 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -3083,13 +3109,13 @@
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3097,13 +3123,13 @@
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3111,13 +3137,13 @@
     </row>
     <row r="8" spans="1:4" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D8" s="19">
         <v>1</v>
@@ -3125,13 +3151,13 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3139,13 +3165,13 @@
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D10" s="19">
         <v>1</v>
@@ -3153,13 +3179,13 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D11" s="19">
         <v>1</v>
@@ -3167,13 +3193,13 @@
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D12" s="19">
         <v>1</v>
@@ -3181,13 +3207,13 @@
     </row>
     <row r="13" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="D13" s="19">
         <v>1</v>
@@ -3195,13 +3221,13 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D14" s="19">
         <v>1</v>
@@ -3209,13 +3235,13 @@
     </row>
     <row r="15" spans="1:4" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D15" s="19">
         <v>1</v>
@@ -3223,13 +3249,13 @@
     </row>
     <row r="16" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D16" s="19">
         <v>1</v>
@@ -3237,13 +3263,13 @@
     </row>
     <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
@@ -3251,13 +3277,13 @@
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D18" s="19">
         <v>1</v>
@@ -3265,13 +3291,13 @@
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D19" s="19">
         <v>1</v>
@@ -3279,13 +3305,13 @@
     </row>
     <row r="20" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D20" s="19">
         <v>1</v>
@@ -3293,13 +3319,13 @@
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="D21" s="19">
         <v>2</v>
@@ -3307,13 +3333,13 @@
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -3321,13 +3347,13 @@
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D23" s="19">
         <v>2</v>
@@ -3335,13 +3361,13 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D24" s="19">
         <v>2</v>
@@ -3349,27 +3375,27 @@
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D25" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D26" s="19">
         <v>2</v>
@@ -3377,13 +3403,13 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D27" s="19">
         <v>2</v>
@@ -3391,13 +3417,13 @@
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D28" s="19">
         <v>2</v>
@@ -3405,13 +3431,13 @@
     </row>
     <row r="29" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -3419,13 +3445,13 @@
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -3433,27 +3459,27 @@
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -3461,13 +3487,13 @@
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -3475,13 +3501,13 @@
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -3489,13 +3515,13 @@
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -3503,13 +3529,13 @@
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -3517,13 +3543,13 @@
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -3531,13 +3557,13 @@
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -3545,13 +3571,13 @@
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D39" s="19">
         <v>3</v>
@@ -3559,13 +3585,13 @@
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D40" s="19">
         <v>3</v>
@@ -3573,13 +3599,13 @@
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D41" s="19">
         <v>3</v>
@@ -3587,13 +3613,13 @@
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -3601,13 +3627,13 @@
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D43">
         <v>3</v>

</xml_diff>

<commit_message>
Updated stories and tasks for sprint 1
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\ssw555tm022018Spring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Desktop\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="212">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -675,13 +675,37 @@
     <t>Act Time (mins)</t>
   </si>
   <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
     <t>Database:</t>
   </si>
   <si>
     <t>sqLite3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complete </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>T3.1</t>
+  </si>
+  <si>
+    <t>T3.2</t>
+  </si>
+  <si>
+    <t>T3.3</t>
+  </si>
+  <si>
+    <t>method for checking if there is a death date</t>
+  </si>
+  <si>
+    <t>if there is a death date take the difference of the death date and the birthdate</t>
+  </si>
+  <si>
+    <t>if negative print error statement</t>
   </si>
 </sst>
 </file>
@@ -944,28 +968,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -983,21 +986,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF5050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2088,17 +2077,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.4609375" customWidth="1"/>
-    <col min="3" max="3" width="9.61328125" customWidth="1"/>
-    <col min="4" max="4" width="20.4609375" customWidth="1"/>
-    <col min="5" max="5" width="47.3828125" customWidth="1"/>
+    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.46875" customWidth="1"/>
+    <col min="3" max="3" width="9.5859375" customWidth="1"/>
+    <col min="4" max="4" width="20.46875" customWidth="1"/>
+    <col min="5" max="5" width="47.3515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2135,7 +2124,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2178,10 +2167,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D13" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>202</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2202,17 +2191,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.84375" customWidth="1"/>
-    <col min="2" max="2" width="22.61328125" customWidth="1"/>
-    <col min="3" max="3" width="38.15234375" customWidth="1"/>
-    <col min="4" max="4" width="8.07421875" customWidth="1"/>
-    <col min="5" max="5" width="7.61328125" customWidth="1"/>
+    <col min="1" max="1" width="8.8203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5859375" customWidth="1"/>
+    <col min="3" max="3" width="38.17578125" customWidth="1"/>
+    <col min="4" max="4" width="8.05859375" customWidth="1"/>
+    <col min="5" max="5" width="7.5859375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2417,14 +2406,14 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3828125" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.8203125" style="7"/>
+    <col min="2" max="2" width="9.46875" customWidth="1"/>
+    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3515625" customWidth="1"/>
+    <col min="5" max="5" width="6.8203125" customWidth="1"/>
+    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2611,14 +2600,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="16.61328125" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.8203125" style="2"/>
+    <col min="2" max="2" width="16.5859375" customWidth="1"/>
+    <col min="3" max="3" width="12.46875" customWidth="1"/>
+    <col min="4" max="4" width="7.17578125" customWidth="1"/>
+    <col min="5" max="5" width="6.8203125" customWidth="1"/>
+    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2679,22 +2668,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.61328125" customWidth="1"/>
-    <col min="2" max="2" width="29.23046875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.61328125" customWidth="1"/>
-    <col min="5" max="5" width="13.3828125" customWidth="1"/>
-    <col min="6" max="6" width="15.84375" customWidth="1"/>
-    <col min="7" max="7" width="20.23046875" customWidth="1"/>
-    <col min="8" max="8" width="21.53515625" customWidth="1"/>
-    <col min="9" max="9" width="14.69140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="7.5859375" customWidth="1"/>
+    <col min="2" max="2" width="29.234375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5859375" customWidth="1"/>
+    <col min="5" max="5" width="14.52734375" customWidth="1"/>
+    <col min="6" max="6" width="15.8203125" customWidth="1"/>
+    <col min="7" max="7" width="20.234375" customWidth="1"/>
+    <col min="8" max="8" width="21.52734375" customWidth="1"/>
+    <col min="9" max="9" width="14.703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2726,7 +2715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -2737,13 +2726,22 @@
         <v>195</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E2">
         <v>35</v>
       </c>
       <c r="F2">
         <v>45</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2760,7 +2758,7 @@
         <v>192</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -2780,7 +2778,7 @@
         <v>192</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -2789,74 +2787,100 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>116</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6">
+      <c r="D8" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8">
         <v>65</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="9" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="37.15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>117</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B12" t="s">
         <v>70</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C12" t="s">
         <v>193</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7">
+      <c r="D12" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="E12">
         <v>65</v>
       </c>
-      <c r="F7">
+      <c r="F12">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="7"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="5"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2DCD5CA0-4A5A-4BD1-984B-70D227AFE942}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",D1)))</formula>
-    </cfRule>
+  <conditionalFormatting sqref="D1:D5 D8 D10:D1048576">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2876,7 +2900,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D1:D1048576</xm:sqref>
+          <xm:sqref>D1:D5 D8 D10:D1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2892,9 +2916,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2938,9 +2962,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2983,9 +3007,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3025,15 +3049,15 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:C20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.23046875" customWidth="1"/>
-    <col min="2" max="2" width="30.765625" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.234375" customWidth="1"/>
+    <col min="2" max="2" width="30.76171875" customWidth="1"/>
+    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3387,7 +3411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
framework for test suite started -- tests still need to be defined minor updates to team report
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="214">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -706,6 +706,12 @@
   </si>
   <si>
     <t>if negative print error statement</t>
+  </si>
+  <si>
+    <t>T5.0</t>
+  </si>
+  <si>
+    <t>begin developing automated testing suite</t>
   </si>
 </sst>
 </file>
@@ -2191,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2231,6 +2237,9 @@
       <c r="C2" s="12" t="s">
         <v>35</v>
       </c>
+      <c r="D2" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2242,6 +2251,9 @@
       <c r="C3" s="12" t="s">
         <v>36</v>
       </c>
+      <c r="D3" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2253,6 +2265,9 @@
       <c r="C4" s="12" t="s">
         <v>37</v>
       </c>
+      <c r="D4" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2263,6 +2278,9 @@
       </c>
       <c r="C5" s="12" t="s">
         <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.3">
@@ -2670,8 +2688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2849,6 +2867,26 @@
       </c>
       <c r="F12">
         <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E14">
+        <v>75</v>
+      </c>
+      <c r="F14">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated for current sprint, minor planning for sprint 2
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="211">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -657,9 +657,6 @@
     <t>T0.0</t>
   </si>
   <si>
-    <t>DC/NO</t>
-  </si>
-  <si>
     <t>develop date conversion method to be used in stories for this sprint</t>
   </si>
   <si>
@@ -681,37 +678,31 @@
     <t>sqLite3</t>
   </si>
   <si>
-    <t xml:space="preserve">complete </t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>in progress</t>
   </si>
   <si>
-    <t>T3.1</t>
-  </si>
-  <si>
-    <t>T3.2</t>
-  </si>
-  <si>
-    <t>T3.3</t>
-  </si>
-  <si>
-    <t>method for checking if there is a death date</t>
-  </si>
-  <si>
-    <t>if there is a death date take the difference of the death date and the birthdate</t>
-  </si>
-  <si>
-    <t>if negative print error statement</t>
-  </si>
-  <si>
-    <t>T5.0</t>
-  </si>
-  <si>
-    <t>begin developing automated testing suite</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Refactor GEDCOM Parser</t>
+  </si>
+  <si>
+    <t>T0.1</t>
+  </si>
+  <si>
+    <t>T0.2</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>develop automated testing file</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -866,7 +857,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -905,6 +896,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -974,7 +968,91 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1183,6 +1261,9 @@
                 <c:pt idx="0">
                   <c:v>41681</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>41695</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1194,6 +1275,9 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2173,10 +2257,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D13" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>201</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2197,8 +2281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2240,6 +2324,9 @@
       <c r="D2" t="s">
         <v>192</v>
       </c>
+      <c r="E2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2254,6 +2341,9 @@
       <c r="D3" t="s">
         <v>192</v>
       </c>
+      <c r="E3" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2282,6 +2372,9 @@
       <c r="D5" t="s">
         <v>193</v>
       </c>
+      <c r="E5" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2293,6 +2386,9 @@
       <c r="C6" s="12" t="s">
         <v>39</v>
       </c>
+      <c r="D6" s="18" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2304,6 +2400,9 @@
       <c r="C7" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="D7" s="18" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2315,6 +2414,9 @@
       <c r="C8" s="12" t="s">
         <v>46</v>
       </c>
+      <c r="D8" s="18" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2325,6 +2427,9 @@
       </c>
       <c r="C9" s="12" t="s">
         <v>89</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.3">
@@ -2614,8 +2719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2660,20 +2765,25 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
+      <c r="A3" s="23">
+        <v>41695</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <v>480</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <v>265</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>108.67924528301887</v>
       </c>
     </row>
   </sheetData>
@@ -2686,10 +2796,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2718,16 +2828,16 @@
         <v>12</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>17</v>
@@ -2738,13 +2848,13 @@
         <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="E2">
         <v>35</v>
@@ -2759,44 +2869,79 @@
         <v>60</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D3" s="18"/>
+      <c r="A3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3">
+        <v>120</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" t="s">
-        <v>156</v>
+        <v>207</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>192</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>160</v>
+      </c>
+      <c r="H4">
+        <v>95</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
         <v>192</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -2804,120 +2949,120 @@
       <c r="F5">
         <v>25</v>
       </c>
+      <c r="G5">
+        <v>75</v>
+      </c>
+      <c r="H5">
+        <v>35</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>193</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E8">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="F8">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>206</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="37.15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>207</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="E12">
-        <v>65</v>
-      </c>
-      <c r="F12">
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>212</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C14" t="s">
-        <v>195</v>
-      </c>
-      <c r="D14" t="s">
-        <v>205</v>
-      </c>
-      <c r="E14">
-        <v>75</v>
-      </c>
-      <c r="F14">
-        <v>75</v>
-      </c>
+      <c r="I8" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I15" s="7"/>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2DCD5CA0-4A5A-4BD1-984B-70D227AFE942}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D1:D5 D8 D10:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Incomplete">
+  <conditionalFormatting sqref="D18:D1048576 D16 D13:D14 D1:D8">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2927,9 +3072,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{06A7FB0F-FD25-4481-873C-BCA5B754C452}">
-            <xm:f>NOT(ISERROR(SEARCH("Complete",D1)))</xm:f>
-            <xm:f>"Complete"</xm:f>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{FB5F0E68-4BA8-460F-813D-C6B1A5B5A2AB}">
+            <xm:f>NOT(ISERROR(SEARCH("done",D1)))</xm:f>
+            <xm:f>"done"</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2938,7 +3083,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D1:D5 D8 D10:D1048576</xm:sqref>
+          <xm:sqref>D18:D1048576 D16 D13:D14 D1:D8</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2948,13 +3093,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.17578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
@@ -2983,6 +3131,74 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for end of sprint 1 (conducted sprint review and acceptance test), and planned sprint 2
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Desktop\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EF06E2-DFC4-4789-8DE9-2EE59F26CEA5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,6 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sprint1!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sprint2!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Stories!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="215">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -102,14 +104,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Act Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Completed</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -687,31 +681,40 @@
     <t>yes</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
-    <t>T3.1</t>
-  </si>
-  <si>
-    <t>T3.2</t>
-  </si>
-  <si>
-    <t>T3.3</t>
-  </si>
-  <si>
-    <t>method for checking if there is a death date</t>
-  </si>
-  <si>
-    <t>if there is a death date take the difference of the death date and the birthdate</t>
-  </si>
-  <si>
-    <t>if negative print error statement</t>
-  </si>
-  <si>
-    <t>T5.0</t>
-  </si>
-  <si>
     <t>begin developing automated testing suite</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>- pair programming/screen shares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- concurrent git commits </t>
+  </si>
+  <si>
+    <t>- Test Driven Development</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>T0.1</t>
+  </si>
+  <si>
+    <t>- Use checks in database code for User stories</t>
+  </si>
+  <si>
+    <t>- weekly meetings</t>
+  </si>
+  <si>
+    <t>- after class catch up</t>
+  </si>
+  <si>
+    <t>- avoid multiple instances of radical refactoring</t>
   </si>
 </sst>
 </file>
@@ -974,7 +977,28 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1183,6 +1207,9 @@
                 <c:pt idx="0">
                   <c:v>41681</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>41695</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1194,6 +1221,9 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2098,85 +2128,85 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D11" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D12" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D13" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2197,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2212,196 +2242,220 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>190</v>
+      </c>
+      <c r="E2" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>192</v>
+        <v>190</v>
+      </c>
+      <c r="E3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+      <c r="E5" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2436,37 +2490,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -2478,18 +2532,18 @@
         <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="G14" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2505,7 +2559,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -2530,7 +2584,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -2555,7 +2609,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -2580,7 +2634,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -2615,7 +2669,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2639,13 +2693,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="F1" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2660,20 +2714,25 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
+      <c r="A3" s="23">
+        <v>41695</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <v>80</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <v>255</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>18.823529411764707</v>
       </c>
     </row>
   </sheetData>
@@ -2686,10 +2745,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2718,33 +2777,33 @@
         <v>12</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>200</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E2">
         <v>35</v>
@@ -2759,24 +2818,50 @@
         <v>60</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D3" s="18"/>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3">
+        <v>75</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -2784,19 +2869,28 @@
       <c r="F4">
         <v>25</v>
       </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -2804,93 +2898,112 @@
       <c r="F5">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>120</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="s">
-        <v>193</v>
-      </c>
-      <c r="D8" s="18" t="s">
+      <c r="C7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7">
+        <v>65</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E8">
-        <v>65</v>
-      </c>
-      <c r="F8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>206</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="37.15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="15" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="E12">
-        <v>65</v>
-      </c>
-      <c r="F12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C14" t="s">
-        <v>195</v>
-      </c>
-      <c r="D14" t="s">
-        <v>205</v>
-      </c>
-      <c r="E14">
-        <v>75</v>
-      </c>
-      <c r="F14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I15" s="7"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
@@ -2898,26 +3011,23 @@
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
-        <v>32</v>
+      <c r="B20" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{2DCD5CA0-4A5A-4BD1-984B-70D227AFE942}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D1:D5 D8 D10:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Incomplete">
+  <conditionalFormatting sqref="D15:D1048576 D13 D1:D7">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2938,7 +3048,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D1:D5 D8 D10:D1048576</xm:sqref>
+          <xm:sqref>D15:D1048576 D13 D1:D7</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2948,47 +3058,164 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.05859375" customWidth="1"/>
+    <col min="5" max="5" width="15.52734375" customWidth="1"/>
+    <col min="6" max="6" width="16.05859375" customWidth="1"/>
+    <col min="7" max="7" width="14.9375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>17</v>
+      <c r="F2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{B8883D59-E29E-4833-ABC2-F6D5483C07D2}"/>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D1">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Incomplete">
+      <formula>NOT(ISERROR(SEARCH("Incomplete",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{86CFB130-C427-4945-858F-FFC61254B7FF}">
+            <xm:f>NOT(ISERROR(SEARCH("Complete",D1)))</xm:f>
+            <xm:f>"Complete"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D1</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2996,7 +3223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -3028,7 +3255,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3073,7 +3300,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3101,27 +3328,27 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3129,13 +3356,13 @@
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3143,13 +3370,13 @@
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3157,13 +3384,13 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -3171,13 +3398,13 @@
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3185,13 +3412,13 @@
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3199,13 +3426,13 @@
     </row>
     <row r="8" spans="1:4" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" s="19">
         <v>1</v>
@@ -3213,13 +3440,13 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3227,13 +3454,13 @@
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="19">
         <v>1</v>
@@ -3241,13 +3468,13 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="19">
         <v>1</v>
@@ -3255,13 +3482,13 @@
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D12" s="19">
         <v>1</v>
@@ -3269,13 +3496,13 @@
     </row>
     <row r="13" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D13" s="19">
         <v>1</v>
@@ -3283,13 +3510,13 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D14" s="19">
         <v>1</v>
@@ -3297,13 +3524,13 @@
     </row>
     <row r="15" spans="1:4" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" s="19">
         <v>1</v>
@@ -3311,13 +3538,13 @@
     </row>
     <row r="16" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="19">
         <v>1</v>
@@ -3325,13 +3552,13 @@
     </row>
     <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
@@ -3339,13 +3566,13 @@
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D18" s="19">
         <v>1</v>
@@ -3353,13 +3580,13 @@
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" s="19">
         <v>1</v>
@@ -3367,13 +3594,13 @@
     </row>
     <row r="20" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20" s="19">
         <v>1</v>
@@ -3381,13 +3608,13 @@
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D21" s="19">
         <v>2</v>
@@ -3395,13 +3622,13 @@
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -3409,13 +3636,13 @@
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="19">
         <v>2</v>
@@ -3423,13 +3650,13 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" s="19">
         <v>2</v>
@@ -3437,13 +3664,13 @@
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D25" s="19">
         <v>2</v>
@@ -3451,13 +3678,13 @@
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="19">
         <v>2</v>
@@ -3465,13 +3692,13 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D27" s="19">
         <v>2</v>
@@ -3479,13 +3706,13 @@
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" s="19">
         <v>2</v>
@@ -3493,13 +3720,13 @@
     </row>
     <row r="29" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -3507,13 +3734,13 @@
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -3521,27 +3748,27 @@
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -3549,13 +3776,13 @@
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -3563,13 +3790,13 @@
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -3577,13 +3804,13 @@
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -3591,13 +3818,13 @@
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -3605,13 +3832,13 @@
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -3619,13 +3846,13 @@
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -3633,13 +3860,13 @@
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D39" s="19">
         <v>3</v>
@@ -3647,13 +3874,13 @@
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D40" s="19">
         <v>3</v>
@@ -3661,13 +3888,13 @@
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D41" s="19">
         <v>3</v>
@@ -3675,13 +3902,13 @@
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -3689,13 +3916,13 @@
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D43">
         <v>3</v>

</xml_diff>

<commit_message>
Updated team report for sprint 2 finish and planned sprint 3
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Desktop\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A281A5BE-75E9-451E-8614-AB0E467B5E80}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0CD988-C0AD-440A-B09C-2F51BE19CB26}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="221">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -718,6 +718,21 @@
   </si>
   <si>
     <t xml:space="preserve">yes </t>
+  </si>
+  <si>
+    <t>- refactor when necssary</t>
+  </si>
+  <si>
+    <t>- anaomly checks in database code for User Stories</t>
+  </si>
+  <si>
+    <t>- create new classes for test when applicable</t>
+  </si>
+  <si>
+    <t>- large test classes</t>
+  </si>
+  <si>
+    <t>-multiple instances of the same code</t>
   </si>
 </sst>
 </file>
@@ -1213,6 +1228,9 @@
                 <c:pt idx="1">
                   <c:v>41695</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>41711</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1227,6 +1245,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,10 +2249,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2341,6 +2362,9 @@
       <c r="D6" t="s">
         <v>190</v>
       </c>
+      <c r="E6" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2355,6 +2379,9 @@
       <c r="D7" t="s">
         <v>191</v>
       </c>
+      <c r="E7" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2369,6 +2396,9 @@
       <c r="D8" t="s">
         <v>190</v>
       </c>
+      <c r="E8" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2383,6 +2413,9 @@
       <c r="D9" t="s">
         <v>191</v>
       </c>
+      <c r="E9" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2394,6 +2427,9 @@
       <c r="C10" s="12" t="s">
         <v>88</v>
       </c>
+      <c r="D10" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2416,6 +2452,9 @@
       <c r="C12" s="12" t="s">
         <v>51</v>
       </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2427,6 +2466,9 @@
       <c r="C13" s="12" t="s">
         <v>52</v>
       </c>
+      <c r="D13" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2438,6 +2480,9 @@
       <c r="C14" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2460,6 +2505,18 @@
       <c r="C16" s="12" t="s">
         <v>56</v>
       </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{BB66CDFC-80AF-4E87-8631-F06122380131}">
@@ -2477,7 +2534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
@@ -2669,10 +2726,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2738,6 +2795,29 @@
         <v>18.823529411764707</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>41711</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <f>B3-B4</f>
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <f>D3+70</f>
+        <v>150</v>
+      </c>
+      <c r="E4">
+        <v>70</v>
+      </c>
+      <c r="F4" s="9">
+        <f>(D4-D3)/E4*60</f>
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2751,7 +2831,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -3061,11 +3141,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -3220,6 +3300,67 @@
       </c>
       <c r="I5" t="s">
         <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="37.15" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3264,13 +3405,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.46875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
@@ -3299,6 +3443,86 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3357,8 +3581,8 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -3482,269 +3706,269 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="19">
-        <v>1</v>
+      <c r="A9" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="19">
+        <v>170</v>
+      </c>
+      <c r="D11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>87</v>
+      <c r="A12" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="D12" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>88</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="D13" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>47</v>
+        <v>171</v>
       </c>
       <c r="D14" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>48</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="D15" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>49</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="D16" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>173</v>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="D18" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D19" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>141</v>
-      </c>
-      <c r="B20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>52</v>
+      <c r="A20" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="D20" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>169</v>
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="D21" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
+        <v>87</v>
+      </c>
+      <c r="D22" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>39</v>
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="D23" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>78</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="D24" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>171</v>
+        <v>48</v>
       </c>
       <c r="D25" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>40</v>
+      <c r="A26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="D26" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>44</v>
+        <v>172</v>
       </c>
       <c r="D27" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.3">
@@ -3762,70 +3986,70 @@
       </c>
     </row>
     <row r="29" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>142</v>
-      </c>
-      <c r="B29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
+      <c r="A29" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="D30" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="D31" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -3833,27 +4057,27 @@
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>58</v>
+        <v>100</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="D34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -3861,13 +4085,13 @@
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -3875,13 +4099,13 @@
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -3889,69 +4113,69 @@
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D40" s="19">
-        <v>3</v>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="19">
-        <v>3</v>
+        <v>107</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -3959,22 +4183,22 @@
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{35456034-6B53-4C1C-A5CB-2274B96A163E}">
     <sortState ref="A2:D43">
-      <sortCondition ref="D1"/>
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated backlog and sprint 3 review, planned sprint 4
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4299DCB-6083-4541-9D51-C35DC3FC02DB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC9D974-E203-4DDD-9FD6-B98A62FB3933}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sprint2!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Stories!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="234">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -739,6 +739,39 @@
   </si>
   <si>
     <t>~</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - refactor when necessary</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - TDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - create new classes for test cases when applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - weekly meetings</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - after class catch up</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - dramatic refactoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - wearing selves out trying to solve a problem</t>
+  </si>
+  <si>
+    <t>Unique name and birth</t>
+  </si>
+  <si>
+    <t>incomplete</t>
+  </si>
+  <si>
+    <t>order siublings by age</t>
   </si>
 </sst>
 </file>
@@ -893,7 +926,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -932,6 +965,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2143,7 +2180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -3411,15 +3448,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.4609375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3567,21 +3604,80 @@
         <v>176</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="B14" s="24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="25" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="27" x14ac:dyDescent="0.3">
+      <c r="B20" s="24" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.07421875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
@@ -3609,6 +3705,86 @@
         <v>8</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed burndown chart and other small things from previous sprints
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC9D974-E203-4DDD-9FD6-B98A62FB3933}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A17471-4DEF-4A63-B81F-94BFCACC1C38}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="231">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -699,9 +699,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>pending</t>
-  </si>
-  <si>
     <t>T0.1</t>
   </si>
   <si>
@@ -733,12 +730,6 @@
   </si>
   <si>
     <t>-multiple instances of the same code</t>
-  </si>
-  <si>
-    <t>~30</t>
-  </si>
-  <si>
-    <t>~</t>
   </si>
   <si>
     <t xml:space="preserve"> - refactor when necessary</t>
@@ -1274,6 +1265,9 @@
                 <c:pt idx="2">
                   <c:v>41711</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>41730</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1291,6 +1285,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2294,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -2473,6 +2470,9 @@
       <c r="D10" t="s">
         <v>190</v>
       </c>
+      <c r="E10" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2484,6 +2484,9 @@
       <c r="C11" s="12" t="s">
         <v>47</v>
       </c>
+      <c r="D11" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2498,6 +2501,9 @@
       <c r="D12" t="s">
         <v>191</v>
       </c>
+      <c r="E12" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2512,6 +2518,9 @@
       <c r="D13" t="s">
         <v>191</v>
       </c>
+      <c r="E13" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2526,6 +2535,9 @@
       <c r="D14" t="s">
         <v>190</v>
       </c>
+      <c r="E14" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2537,6 +2549,9 @@
       <c r="C15" s="12" t="s">
         <v>55</v>
       </c>
+      <c r="D15" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2548,6 +2563,9 @@
       <c r="C16" s="12" t="s">
         <v>56</v>
       </c>
+      <c r="D16" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
@@ -2559,7 +2577,9 @@
       <c r="C17" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="19" t="s">
+        <v>190</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{BB66CDFC-80AF-4E87-8631-F06122380131}">
@@ -2769,10 +2789,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -2859,6 +2879,28 @@
       <c r="F4" s="9">
         <f>(D4-D3)/E4*60</f>
         <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>41730</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f>D4+80</f>
+        <v>230</v>
+      </c>
+      <c r="E5">
+        <v>125</v>
+      </c>
+      <c r="F5" s="9">
+        <f>(D5-D4)/E5*60</f>
+        <v>38.4</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +2991,7 @@
     </row>
     <row r="3" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>203</v>
@@ -3117,18 +3159,18 @@
     </row>
     <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
@@ -3143,7 +3185,7 @@
     </row>
     <row r="21" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3188,7 +3230,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3240,7 +3282,7 @@
         <v>190</v>
       </c>
       <c r="D2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -3255,7 +3297,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3269,7 +3311,7 @@
         <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -3284,7 +3326,7 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3298,7 +3340,7 @@
         <v>191</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -3313,7 +3355,7 @@
         <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3327,7 +3369,7 @@
         <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E5">
         <v>35</v>
@@ -3342,7 +3384,7 @@
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -3360,7 +3402,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -3370,17 +3412,17 @@
     </row>
     <row r="17" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
@@ -3393,17 +3435,17 @@
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="40.5" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3451,7 +3493,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3499,7 +3541,7 @@
         <v>190</v>
       </c>
       <c r="D2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -3508,7 +3550,7 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <v>20</v>
@@ -3528,7 +3570,7 @@
         <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -3557,7 +3599,7 @@
         <v>191</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -3572,7 +3614,7 @@
         <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3586,7 +3628,7 @@
         <v>190</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -3594,14 +3636,14 @@
       <c r="F5">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
-        <v>222</v>
-      </c>
-      <c r="H5" t="s">
-        <v>221</v>
+      <c r="G5">
+        <v>35</v>
+      </c>
+      <c r="H5">
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3616,32 +3658,32 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="25" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="25" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
@@ -3651,12 +3693,12 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="25" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3670,7 +3712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -3679,7 +3721,7 @@
     <col min="2" max="2" width="21.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3713,13 +3755,13 @@
         <v>134</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -3739,7 +3781,7 @@
         <v>191</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E3">
         <v>35</v>
@@ -3759,7 +3801,7 @@
         <v>190</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -3773,13 +3815,13 @@
         <v>139</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>190</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E5">
         <v>15</v>

</xml_diff>

<commit_message>
updated team report for work done on 4/3/18 -- suck it
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\ssw555tm022018Spring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Desktop\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A17471-4DEF-4A63-B81F-94BFCACC1C38}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EF3C80-F731-4962-BD92-E4C7331CB8B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="231">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -762,7 +762,7 @@
     <t>incomplete</t>
   </si>
   <si>
-    <t>order siublings by age</t>
+    <t>order siblings by age</t>
   </si>
 </sst>
 </file>
@@ -2181,13 +2181,13 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.4609375" customWidth="1"/>
-    <col min="3" max="3" width="9.61328125" customWidth="1"/>
-    <col min="4" max="4" width="20.4609375" customWidth="1"/>
-    <col min="5" max="5" width="47.3828125" customWidth="1"/>
+    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.46875" customWidth="1"/>
+    <col min="3" max="3" width="9.5859375" customWidth="1"/>
+    <col min="4" max="4" width="20.46875" customWidth="1"/>
+    <col min="5" max="5" width="47.3515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2224,7 +2224,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -2291,17 +2291,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.84375" customWidth="1"/>
-    <col min="2" max="2" width="22.61328125" customWidth="1"/>
-    <col min="3" max="3" width="38.15234375" customWidth="1"/>
-    <col min="4" max="4" width="8.07421875" customWidth="1"/>
-    <col min="5" max="5" width="7.61328125" customWidth="1"/>
+    <col min="1" max="1" width="8.8203125" customWidth="1"/>
+    <col min="2" max="2" width="28.76171875" customWidth="1"/>
+    <col min="3" max="3" width="38.17578125" customWidth="1"/>
+    <col min="4" max="4" width="8.05859375" customWidth="1"/>
+    <col min="5" max="5" width="7.5859375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2487,6 +2487,9 @@
       <c r="D11" t="s">
         <v>191</v>
       </c>
+      <c r="E11" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2551,6 +2554,9 @@
       </c>
       <c r="D15" t="s">
         <v>191</v>
+      </c>
+      <c r="E15" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.3">
@@ -2601,14 +2607,14 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3828125" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.8203125" style="7"/>
+    <col min="2" max="2" width="9.46875" customWidth="1"/>
+    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3515625" customWidth="1"/>
+    <col min="5" max="5" width="6.8203125" customWidth="1"/>
+    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2795,14 +2801,14 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="16.61328125" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.8203125" style="2"/>
+    <col min="2" max="2" width="16.5859375" customWidth="1"/>
+    <col min="3" max="3" width="12.46875" customWidth="1"/>
+    <col min="4" max="4" width="7.17578125" customWidth="1"/>
+    <col min="5" max="5" width="6.8203125" customWidth="1"/>
+    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2919,16 +2925,16 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.61328125" customWidth="1"/>
-    <col min="2" max="2" width="29.23046875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.61328125" customWidth="1"/>
-    <col min="5" max="5" width="14.53515625" customWidth="1"/>
-    <col min="6" max="6" width="15.84375" customWidth="1"/>
-    <col min="7" max="7" width="20.23046875" customWidth="1"/>
-    <col min="8" max="8" width="21.53515625" customWidth="1"/>
-    <col min="9" max="9" width="14.69140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="7.5859375" customWidth="1"/>
+    <col min="2" max="2" width="29.234375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5859375" customWidth="1"/>
+    <col min="5" max="5" width="14.52734375" customWidth="1"/>
+    <col min="6" max="6" width="15.8203125" customWidth="1"/>
+    <col min="7" max="7" width="20.234375" customWidth="1"/>
+    <col min="8" max="8" width="21.52734375" customWidth="1"/>
+    <col min="9" max="9" width="14.703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2960,7 +2966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>192</v>
       </c>
@@ -2989,7 +2995,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -3157,7 +3163,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>210</v>
       </c>
@@ -3183,7 +3189,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="27" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>213</v>
       </c>
@@ -3233,13 +3239,13 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.07421875" customWidth="1"/>
-    <col min="5" max="5" width="15.53515625" customWidth="1"/>
-    <col min="6" max="6" width="16.07421875" customWidth="1"/>
-    <col min="7" max="7" width="14.921875" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" customWidth="1"/>
+    <col min="2" max="2" width="23.05859375" customWidth="1"/>
+    <col min="5" max="5" width="15.52734375" customWidth="1"/>
+    <col min="6" max="6" width="16.05859375" customWidth="1"/>
+    <col min="7" max="7" width="14.9375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3410,7 +3416,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="27" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>217</v>
       </c>
@@ -3438,12 +3444,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="37.15" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="27" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>219</v>
       </c>
@@ -3496,7 +3502,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
@@ -3666,7 +3672,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="37.15" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
         <v>222</v>
       </c>
@@ -3696,7 +3702,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="27" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
         <v>227</v>
       </c>
@@ -3712,13 +3718,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.07421875" customWidth="1"/>
+    <col min="2" max="2" width="21.05859375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3769,6 +3775,15 @@
       <c r="F2">
         <v>15</v>
       </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -3789,6 +3804,15 @@
       <c r="F3">
         <v>30</v>
       </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -3828,6 +3852,15 @@
       </c>
       <c r="F5">
         <v>15</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3845,11 +3878,11 @@
       <selection pane="bottomLeft" activeCell="A29" sqref="A29:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.23046875" customWidth="1"/>
-    <col min="2" max="2" width="30.765625" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.234375" customWidth="1"/>
+    <col min="2" max="2" width="30.76171875" customWidth="1"/>
+    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4049,7 +4082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>125</v>
       </c>
@@ -4329,7 +4362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
updated product backlog completion status as well as sprint 4 completion status and actual metrics for LOC and effort.
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Desktop\ssw555tm022018Spring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EF3C80-F731-4962-BD92-E4C7331CB8B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B400DE17-A97E-41EE-873B-5E37F56DDA45}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15383" windowHeight="8963" tabRatio="594" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="231">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -917,7 +917,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -960,6 +960,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2181,13 +2182,13 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.46875" customWidth="1"/>
-    <col min="3" max="3" width="9.5859375" customWidth="1"/>
-    <col min="4" max="4" width="20.46875" customWidth="1"/>
-    <col min="5" max="5" width="47.3515625" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.4609375" customWidth="1"/>
+    <col min="3" max="3" width="9.61328125" customWidth="1"/>
+    <col min="4" max="4" width="20.4609375" customWidth="1"/>
+    <col min="5" max="5" width="47.3828125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2224,7 +2225,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -2291,17 +2292,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.8203125" customWidth="1"/>
-    <col min="2" max="2" width="28.76171875" customWidth="1"/>
-    <col min="3" max="3" width="38.17578125" customWidth="1"/>
-    <col min="4" max="4" width="8.05859375" customWidth="1"/>
-    <col min="5" max="5" width="7.5859375" customWidth="1"/>
+    <col min="1" max="1" width="8.84375" customWidth="1"/>
+    <col min="2" max="2" width="28.765625" customWidth="1"/>
+    <col min="3" max="3" width="38.15234375" customWidth="1"/>
+    <col min="4" max="4" width="8.07421875" customWidth="1"/>
+    <col min="5" max="5" width="7.61328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2572,8 +2573,11 @@
       <c r="D16" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>139</v>
       </c>
@@ -2585,6 +2589,9 @@
       </c>
       <c r="D17" s="19" t="s">
         <v>190</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2607,14 +2614,14 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="7"/>
-    <col min="2" max="2" width="9.46875" customWidth="1"/>
-    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3515625" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="7"/>
+    <col min="2" max="2" width="9.4609375" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3828125" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2801,14 +2808,14 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="2"/>
-    <col min="2" max="2" width="16.5859375" customWidth="1"/>
-    <col min="3" max="3" width="12.46875" customWidth="1"/>
-    <col min="4" max="4" width="7.17578125" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="2"/>
+    <col min="2" max="2" width="16.61328125" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2925,16 +2932,16 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5859375" customWidth="1"/>
-    <col min="2" max="2" width="29.234375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5859375" customWidth="1"/>
-    <col min="5" max="5" width="14.52734375" customWidth="1"/>
-    <col min="6" max="6" width="15.8203125" customWidth="1"/>
-    <col min="7" max="7" width="20.234375" customWidth="1"/>
-    <col min="8" max="8" width="21.52734375" customWidth="1"/>
-    <col min="9" max="9" width="14.703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="7.61328125" customWidth="1"/>
+    <col min="2" max="2" width="29.23046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.61328125" customWidth="1"/>
+    <col min="5" max="5" width="14.53515625" customWidth="1"/>
+    <col min="6" max="6" width="15.84375" customWidth="1"/>
+    <col min="7" max="7" width="20.23046875" customWidth="1"/>
+    <col min="8" max="8" width="21.53515625" customWidth="1"/>
+    <col min="9" max="9" width="14.69140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2966,7 +2973,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>192</v>
       </c>
@@ -2995,7 +3002,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -3163,7 +3170,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>210</v>
       </c>
@@ -3189,7 +3196,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>213</v>
       </c>
@@ -3239,13 +3246,13 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.05859375" customWidth="1"/>
-    <col min="5" max="5" width="15.52734375" customWidth="1"/>
-    <col min="6" max="6" width="16.05859375" customWidth="1"/>
-    <col min="7" max="7" width="14.9375" customWidth="1"/>
-    <col min="8" max="8" width="16.234375" customWidth="1"/>
+    <col min="2" max="2" width="23.07421875" customWidth="1"/>
+    <col min="5" max="5" width="15.53515625" customWidth="1"/>
+    <col min="6" max="6" width="16.07421875" customWidth="1"/>
+    <col min="7" max="7" width="14.921875" customWidth="1"/>
+    <col min="8" max="8" width="16.23046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3416,7 +3423,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>217</v>
       </c>
@@ -3444,12 +3451,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="37.15" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="40.5" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>219</v>
       </c>
@@ -3502,7 +3509,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
@@ -3672,7 +3679,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="37.15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
         <v>222</v>
       </c>
@@ -3702,7 +3709,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
         <v>227</v>
       </c>
@@ -3719,15 +3726,15 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.05859375" customWidth="1"/>
+    <col min="2" max="2" width="21.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="12.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3756,7 +3763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="12.4" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>134</v>
       </c>
@@ -3811,7 +3818,7 @@
         <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3832,6 +3839,15 @@
       </c>
       <c r="F4">
         <v>25</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4" s="26">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3878,11 +3894,11 @@
       <selection pane="bottomLeft" activeCell="A29" sqref="A29:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.234375" customWidth="1"/>
-    <col min="2" max="2" width="30.76171875" customWidth="1"/>
-    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.23046875" customWidth="1"/>
+    <col min="2" max="2" width="30.765625" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4082,7 +4098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>125</v>
       </c>
@@ -4362,7 +4378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
updated team report for sprint 4 completion
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesto\Documents\ssw555tm022018Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B400DE17-A97E-41EE-873B-5E37F56DDA45}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F1041D-23A2-40ED-B30E-88C9D3EE618A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="8960" tabRatio="594" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="241">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -763,6 +763,36 @@
   </si>
   <si>
     <t>order siblings by age</t>
+  </si>
+  <si>
+    <t>NOTE** Restrospective Based on what we would do in future projects</t>
+  </si>
+  <si>
+    <t>Avoid Next time</t>
+  </si>
+  <si>
+    <t>- Use a continuous intergration tool to manage builds</t>
+  </si>
+  <si>
+    <t>- jumping into an architecture based on the user stories of the first sprint</t>
+  </si>
+  <si>
+    <t>- plan before executing each sprint</t>
+  </si>
+  <si>
+    <t>Do Next time/continue doing</t>
+  </si>
+  <si>
+    <t>- pair programming</t>
+  </si>
+  <si>
+    <t>- work in a bigger team to get a better feel for how XP really works</t>
+  </si>
+  <si>
+    <t>- refactoring mid sprint</t>
+  </si>
+  <si>
+    <t>- test to make sure code works before pushing</t>
   </si>
 </sst>
 </file>
@@ -917,7 +947,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -961,6 +991,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1269,6 +1302,9 @@
                 <c:pt idx="3">
                   <c:v>41730</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>41732</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1289,6 +1325,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2802,10 +2841,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -2914,6 +2953,28 @@
       <c r="F5" s="9">
         <f>(D5-D4)/E5*60</f>
         <v>38.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>41732</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <f>D5+100</f>
+        <v>330</v>
+      </c>
+      <c r="E6">
+        <v>110</v>
+      </c>
+      <c r="F6" s="9">
+        <f>(D6-D5)/E6*60</f>
+        <v>54.545454545454547</v>
       </c>
     </row>
   </sheetData>
@@ -3506,7 +3567,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3723,10 +3784,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3734,7 +3795,7 @@
     <col min="2" max="2" width="21.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3763,7 +3824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>134</v>
       </c>
@@ -3877,6 +3938,72 @@
       </c>
       <c r="I5" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="27" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="54" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="e">
+        <f>- pushing broken code</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>